<commit_message>
Update value set template to align with lates from VSAC
-Added 'code system' row and 'Expansion Version' rows
</commit_message>
<xml_diff>
--- a/codevalidator-api/docs/ValueSet_format_Template.xlsx
+++ b/codevalidator-api/docs/ValueSet_format_Template.xlsx
@@ -5,23 +5,23 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AIadministrator\git\codevalidator\codevalidator-api\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ai-vmdc1\RedirectedFolders\amore\Desktop\SITE_VSAC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DD811E80-F793-49A0-8AB0-03C01BEFD139}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{61975850-7EF6-420B-BB27-4DF6BC661BDF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="270" windowWidth="14940" windowHeight="9150"/>
+    <workbookView xWindow="360" yWindow="270" windowWidth="14940" windowHeight="9150" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Value Set Info" sheetId="1" r:id="rId1"/>
     <sheet name="Code List" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511" refMode="R1C1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
   <si>
     <t>Value Set Name</t>
   </si>
@@ -73,12 +73,18 @@
   <si>
     <t>TTY</t>
   </si>
+  <si>
+    <t>Expansion Version</t>
+  </si>
+  <si>
+    <t>Member Information</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -100,6 +106,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="12"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="4">
@@ -149,7 +161,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -162,6 +174,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -516,11 +531,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="14" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -532,73 +547,85 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="5"/>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
+      <c r="A1" s="6"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
     </row>
     <row r="2" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="B4" s="3"/>
+    </row>
+    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="B5" s="3"/>
+    </row>
+    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="3"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="B6" s="3"/>
+    </row>
+    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="3"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B8" s="2"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+      <c r="B10" s="3"/>
+    </row>
+    <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="3"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+      <c r="B11" s="3"/>
+    </row>
+    <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="3"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+      <c r="B12" s="3"/>
+    </row>
+    <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="3"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
+      <c r="B13" s="3"/>
+    </row>
+    <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="3"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+      <c r="B14" s="3"/>
+    </row>
+    <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="3"/>
+    </row>
+    <row r="17" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -616,11 +643,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F823"/>
+  <dimension ref="A1:F825"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="11" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="13" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -633,84 +660,81 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="5"/>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
+      <c r="A1" s="6"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
     </row>
     <row r="2" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="B5" s="3"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="3"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="B6" s="3"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="3"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B8" s="2"/>
+      <c r="B7" s="3"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B9" s="2"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+      <c r="B10" s="2"/>
+    </row>
+    <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
@@ -825,12 +849,16 @@
       <c r="F27" s="4"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
@@ -5599,6 +5627,18 @@
       <c r="D823" s="4"/>
       <c r="E823" s="4"/>
       <c r="F823" s="4"/>
+    </row>
+    <row r="824" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C824" s="4"/>
+      <c r="D824" s="4"/>
+      <c r="E824" s="4"/>
+      <c r="F824" s="4"/>
+    </row>
+    <row r="825" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C825" s="4"/>
+      <c r="D825" s="4"/>
+      <c r="E825" s="4"/>
+      <c r="F825" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>